<commit_message>
Update files to match v1.02
</commit_message>
<xml_diff>
--- a/WorkbookTemplates/Prepare_transform_data_templates/Prepare_Pivot_TimeSeries_data.xlsx
+++ b/WorkbookTemplates/Prepare_transform_data_templates/Prepare_Pivot_TimeSeries_data.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adel\Documents\GitHub\WamdamProject\WaMDaM_UseCases\UseCases_files\0WorkbookTemplates\Prepare_transform_data_templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RC\FinalDatasets_April_2018\Preperation_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11295"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15615" windowHeight="2430"/>
   </bookViews>
   <sheets>
     <sheet name="HomePage" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="56">
   <si>
     <t>Excel sheets to prepare time sereis data for use in WaMDaM</t>
   </si>
@@ -185,9 +185,6 @@
     <t>HomePage!A1</t>
   </si>
   <si>
-    <t xml:space="preserve">Copyright (c) 2017, Utah State University and WaM-DaM development team: </t>
-  </si>
-  <si>
     <t>Adel M. Abdallah and David E. Rosenberg. All rights reserved.</t>
   </si>
   <si>
@@ -213,7 +210,13 @@
 OF THIS SOFTWARE, EVEN IF ADVISED OF THE POSSIBILITY OF SUCH DAMAGE.</t>
   </si>
   <si>
-    <t>WaMDaM V1.0 November 2017</t>
+    <t>WaMDaM V1.02 May 2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Copyright (c) 2018, Utah State University and WaM-DaM development team: </t>
+  </si>
+  <si>
+    <t>wamdam.org</t>
   </si>
 </sst>
 </file>
@@ -748,7 +751,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="4" applyFont="1" applyFill="1" applyProtection="1">
       <protection locked="0"/>
@@ -1049,6 +1052,33 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
@@ -1339,7 +1369,7 @@
   <dimension ref="A1:K56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1353,35 +1383,40 @@
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="28"/>
-      <c r="C1" s="97" t="s">
+      <c r="C1" s="116" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="98"/>
-      <c r="E1" s="98"/>
-      <c r="F1" s="98"/>
-      <c r="G1" s="98"/>
-      <c r="H1" s="98"/>
+      <c r="D1" s="117"/>
+      <c r="E1" s="117"/>
+      <c r="F1" s="117"/>
+      <c r="G1" s="117"/>
+      <c r="H1" s="118"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="28"/>
       <c r="B2" s="97" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="98"/>
-      <c r="G2" s="98"/>
-      <c r="H2" s="98"/>
-      <c r="I2" s="98"/>
+      <c r="C2" s="114"/>
+      <c r="D2" s="114"/>
+      <c r="E2" s="114"/>
+      <c r="F2" s="114"/>
+      <c r="G2" s="114"/>
+      <c r="H2" s="114"/>
+      <c r="I2" s="115"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D3" s="97" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
+      <c r="E3" s="114"/>
+      <c r="F3" s="114"/>
+      <c r="G3" s="115"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E4" s="93" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="5" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -1912,7 +1947,7 @@
   <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6541,7 +6576,7 @@
   <dimension ref="A1:H636"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD636"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14547,7 +14582,7 @@
   <dimension ref="A1:H381"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14599,41 +14634,41 @@
       <c r="A5" s="103" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="107"/>
-      <c r="C5" s="107"/>
-      <c r="D5" s="107"/>
-      <c r="E5" s="107"/>
-      <c r="F5" s="107"/>
-      <c r="G5" s="107"/>
-      <c r="H5" s="107"/>
+      <c r="B5" s="104"/>
+      <c r="C5" s="104"/>
+      <c r="D5" s="104"/>
+      <c r="E5" s="104"/>
+      <c r="F5" s="104"/>
+      <c r="G5" s="104"/>
+      <c r="H5" s="105"/>
     </row>
     <row r="6" spans="1:8" s="95" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="108"/>
-      <c r="B6" s="107"/>
-      <c r="C6" s="107"/>
-      <c r="D6" s="107"/>
-      <c r="E6" s="107"/>
-      <c r="F6" s="107"/>
-      <c r="G6" s="107"/>
-      <c r="H6" s="107"/>
+      <c r="B6" s="104"/>
+      <c r="C6" s="104"/>
+      <c r="D6" s="104"/>
+      <c r="E6" s="104"/>
+      <c r="F6" s="104"/>
+      <c r="G6" s="104"/>
+      <c r="H6" s="105"/>
     </row>
     <row r="7" spans="1:8" s="95" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="34" t="s">
+      <c r="A7" s="119" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="120" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="36" t="s">
+      <c r="C7" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="35" t="s">
+      <c r="D7" s="120" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="35" t="s">
+      <c r="E7" s="120" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="35" t="s">
+      <c r="F7" s="120" t="s">
         <v>29</v>
       </c>
       <c r="G7" s="43" t="s">
@@ -14647,22 +14682,22 @@
       <c r="A8" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="38" t="s">
+      <c r="B8" s="121" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="38" t="s">
+      <c r="C8" s="121" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="38" t="s">
+      <c r="D8" s="121" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="38" t="s">
+      <c r="E8" s="121" t="s">
         <v>38</v>
       </c>
-      <c r="F8" s="38" t="s">
+      <c r="F8" s="121" t="s">
         <v>38</v>
       </c>
-      <c r="G8" s="45" t="s">
+      <c r="G8" s="122" t="s">
         <v>38</v>
       </c>
       <c r="H8" s="30" t="s">
@@ -14673,22 +14708,22 @@
       <c r="A9" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="123" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="52" t="s">
+      <c r="C9" s="124" t="s">
         <v>41</v>
       </c>
-      <c r="D9" s="52" t="s">
+      <c r="D9" s="124" t="s">
         <v>42</v>
       </c>
-      <c r="E9" s="52" t="s">
+      <c r="E9" s="124" t="s">
         <v>43</v>
       </c>
-      <c r="F9" s="52" t="s">
+      <c r="F9" s="124" t="s">
         <v>44</v>
       </c>
-      <c r="G9" s="52" t="s">
+      <c r="G9" s="124" t="s">
         <v>45</v>
       </c>
       <c r="H9" s="53" t="s">
@@ -14696,184 +14731,184 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10"/>
-      <c r="B10"/>
-      <c r="C10"/>
-      <c r="D10"/>
-      <c r="E10"/>
-      <c r="F10"/>
-      <c r="G10"/>
-      <c r="H10"/>
+      <c r="A10" s="73"/>
+      <c r="B10" s="73"/>
+      <c r="C10" s="73"/>
+      <c r="D10" s="73"/>
+      <c r="E10" s="73"/>
+      <c r="F10" s="73"/>
+      <c r="G10" s="73"/>
+      <c r="H10" s="73"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11"/>
-      <c r="B11"/>
-      <c r="C11"/>
-      <c r="D11"/>
-      <c r="E11"/>
-      <c r="F11"/>
-      <c r="G11"/>
-      <c r="H11"/>
+      <c r="A11" s="73"/>
+      <c r="B11" s="73"/>
+      <c r="C11" s="73"/>
+      <c r="D11" s="73"/>
+      <c r="E11" s="73"/>
+      <c r="F11" s="73"/>
+      <c r="G11" s="73"/>
+      <c r="H11" s="73"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12"/>
-      <c r="B12"/>
-      <c r="C12"/>
-      <c r="D12"/>
-      <c r="E12"/>
-      <c r="F12"/>
-      <c r="G12"/>
-      <c r="H12"/>
+      <c r="A12" s="73"/>
+      <c r="B12" s="73"/>
+      <c r="C12" s="73"/>
+      <c r="D12" s="73"/>
+      <c r="E12" s="73"/>
+      <c r="F12" s="73"/>
+      <c r="G12" s="73"/>
+      <c r="H12" s="73"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13"/>
-      <c r="B13"/>
-      <c r="C13"/>
-      <c r="D13"/>
-      <c r="E13"/>
-      <c r="F13"/>
-      <c r="G13"/>
-      <c r="H13"/>
+      <c r="A13" s="73"/>
+      <c r="B13" s="73"/>
+      <c r="C13" s="73"/>
+      <c r="D13" s="73"/>
+      <c r="E13" s="73"/>
+      <c r="F13" s="73"/>
+      <c r="G13" s="73"/>
+      <c r="H13" s="73"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14"/>
-      <c r="B14"/>
-      <c r="C14"/>
-      <c r="D14"/>
-      <c r="E14"/>
-      <c r="F14"/>
-      <c r="G14"/>
-      <c r="H14"/>
+      <c r="A14" s="73"/>
+      <c r="B14" s="73"/>
+      <c r="C14" s="73"/>
+      <c r="D14" s="73"/>
+      <c r="E14" s="73"/>
+      <c r="F14" s="73"/>
+      <c r="G14" s="73"/>
+      <c r="H14" s="73"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15"/>
-      <c r="B15"/>
-      <c r="C15"/>
-      <c r="D15"/>
-      <c r="E15"/>
-      <c r="F15"/>
-      <c r="G15"/>
-      <c r="H15"/>
+      <c r="A15" s="73"/>
+      <c r="B15" s="73"/>
+      <c r="C15" s="73"/>
+      <c r="D15" s="73"/>
+      <c r="E15" s="73"/>
+      <c r="F15" s="73"/>
+      <c r="G15" s="73"/>
+      <c r="H15" s="73"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16"/>
-      <c r="B16"/>
-      <c r="C16"/>
-      <c r="D16"/>
-      <c r="E16"/>
-      <c r="F16"/>
-      <c r="G16"/>
-      <c r="H16"/>
+      <c r="A16" s="73"/>
+      <c r="B16" s="73"/>
+      <c r="C16" s="73"/>
+      <c r="D16" s="73"/>
+      <c r="E16" s="73"/>
+      <c r="F16" s="73"/>
+      <c r="G16" s="73"/>
+      <c r="H16" s="73"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17"/>
-      <c r="B17"/>
-      <c r="C17"/>
-      <c r="D17"/>
-      <c r="E17"/>
-      <c r="F17"/>
-      <c r="G17"/>
-      <c r="H17"/>
+      <c r="A17" s="73"/>
+      <c r="B17" s="73"/>
+      <c r="C17" s="73"/>
+      <c r="D17" s="73"/>
+      <c r="E17" s="73"/>
+      <c r="F17" s="73"/>
+      <c r="G17" s="73"/>
+      <c r="H17" s="73"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18"/>
-      <c r="B18"/>
-      <c r="C18"/>
-      <c r="D18"/>
-      <c r="E18"/>
-      <c r="F18"/>
-      <c r="G18"/>
-      <c r="H18"/>
+      <c r="A18" s="73"/>
+      <c r="B18" s="73"/>
+      <c r="C18" s="73"/>
+      <c r="D18" s="73"/>
+      <c r="E18" s="73"/>
+      <c r="F18" s="73"/>
+      <c r="G18" s="73"/>
+      <c r="H18" s="73"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19"/>
-      <c r="B19"/>
-      <c r="C19"/>
-      <c r="D19"/>
-      <c r="E19"/>
-      <c r="F19"/>
-      <c r="G19"/>
-      <c r="H19"/>
+      <c r="A19" s="73"/>
+      <c r="B19" s="73"/>
+      <c r="C19" s="73"/>
+      <c r="D19" s="73"/>
+      <c r="E19" s="73"/>
+      <c r="F19" s="73"/>
+      <c r="G19" s="73"/>
+      <c r="H19" s="73"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20"/>
-      <c r="B20"/>
-      <c r="C20"/>
-      <c r="D20"/>
-      <c r="E20"/>
-      <c r="F20"/>
-      <c r="G20"/>
-      <c r="H20"/>
+      <c r="A20" s="73"/>
+      <c r="B20" s="73"/>
+      <c r="C20" s="73"/>
+      <c r="D20" s="73"/>
+      <c r="E20" s="73"/>
+      <c r="F20" s="73"/>
+      <c r="G20" s="73"/>
+      <c r="H20" s="73"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21"/>
-      <c r="B21"/>
-      <c r="C21"/>
-      <c r="D21"/>
-      <c r="E21"/>
-      <c r="F21"/>
-      <c r="G21"/>
-      <c r="H21"/>
+      <c r="A21" s="73"/>
+      <c r="B21" s="73"/>
+      <c r="C21" s="73"/>
+      <c r="D21" s="73"/>
+      <c r="E21" s="73"/>
+      <c r="F21" s="73"/>
+      <c r="G21" s="73"/>
+      <c r="H21" s="73"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22"/>
-      <c r="B22"/>
-      <c r="C22"/>
-      <c r="D22"/>
-      <c r="E22"/>
-      <c r="F22"/>
-      <c r="G22"/>
-      <c r="H22"/>
+      <c r="A22" s="73"/>
+      <c r="B22" s="73"/>
+      <c r="C22" s="73"/>
+      <c r="D22" s="73"/>
+      <c r="E22" s="73"/>
+      <c r="F22" s="73"/>
+      <c r="G22" s="73"/>
+      <c r="H22" s="73"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23"/>
-      <c r="B23"/>
-      <c r="C23"/>
-      <c r="D23"/>
-      <c r="E23"/>
-      <c r="F23"/>
-      <c r="G23"/>
-      <c r="H23"/>
+      <c r="A23" s="73"/>
+      <c r="B23" s="73"/>
+      <c r="C23" s="73"/>
+      <c r="D23" s="73"/>
+      <c r="E23" s="73"/>
+      <c r="F23" s="73"/>
+      <c r="G23" s="73"/>
+      <c r="H23" s="73"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24"/>
-      <c r="B24"/>
-      <c r="C24"/>
-      <c r="D24"/>
-      <c r="E24"/>
-      <c r="F24"/>
-      <c r="G24"/>
-      <c r="H24"/>
+      <c r="A24" s="73"/>
+      <c r="B24" s="73"/>
+      <c r="C24" s="73"/>
+      <c r="D24" s="73"/>
+      <c r="E24" s="73"/>
+      <c r="F24" s="73"/>
+      <c r="G24" s="73"/>
+      <c r="H24" s="73"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25"/>
-      <c r="B25"/>
-      <c r="C25"/>
-      <c r="D25"/>
-      <c r="E25"/>
-      <c r="F25"/>
-      <c r="G25"/>
-      <c r="H25"/>
+      <c r="A25" s="73"/>
+      <c r="B25" s="73"/>
+      <c r="C25" s="73"/>
+      <c r="D25" s="73"/>
+      <c r="E25" s="73"/>
+      <c r="F25" s="73"/>
+      <c r="G25" s="73"/>
+      <c r="H25" s="73"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26"/>
-      <c r="B26"/>
-      <c r="C26"/>
-      <c r="D26"/>
-      <c r="E26"/>
-      <c r="F26"/>
-      <c r="G26"/>
-      <c r="H26"/>
+      <c r="A26" s="73"/>
+      <c r="B26" s="73"/>
+      <c r="C26" s="73"/>
+      <c r="D26" s="73"/>
+      <c r="E26" s="73"/>
+      <c r="F26" s="73"/>
+      <c r="G26" s="73"/>
+      <c r="H26" s="73"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27"/>
-      <c r="B27"/>
-      <c r="C27"/>
-      <c r="D27"/>
-      <c r="E27"/>
-      <c r="F27"/>
-      <c r="G27"/>
-      <c r="H27"/>
+      <c r="A27" s="73"/>
+      <c r="B27" s="73"/>
+      <c r="C27" s="73"/>
+      <c r="D27" s="73"/>
+      <c r="E27" s="73"/>
+      <c r="F27" s="73"/>
+      <c r="G27" s="73"/>
+      <c r="H27" s="73"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28"/>
@@ -18433,7 +18468,7 @@
   <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="A5" sqref="A5:L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18453,7 +18488,7 @@
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="109" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B2" s="107"/>
       <c r="C2" s="107"/>
@@ -18469,7 +18504,7 @@
     </row>
     <row r="3" spans="1:12" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="110" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B3" s="107"/>
       <c r="C3" s="107"/>
@@ -18486,7 +18521,7 @@
     <row r="4" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="111" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B5" s="107"/>
       <c r="C5" s="107"/>

</xml_diff>